<commit_message>
updated comments, added retrieval type and correct response
</commit_message>
<xml_diff>
--- a/data/sub-9999/retrieval1.xlsx
+++ b/data/sub-9999/retrieval1.xlsx
@@ -14,11 +14,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="53">
   <si>
     <t>retrieval1</t>
   </si>
   <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>correct</t>
+  </si>
+  <si>
     <t>SetC/001a.jpg</t>
   </si>
   <si>
@@ -161,6 +167,12 @@
   </si>
   <si>
     <t>SetC/048b.jpg</t>
+  </si>
+  <si>
+    <t>targ</t>
+  </si>
+  <si>
+    <t>lure</t>
   </si>
 </sst>
 </file>
@@ -518,255 +530,549 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A49"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
+        <v>28</v>
+      </c>
+      <c r="B27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
+        <v>29</v>
+      </c>
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
+        <v>30</v>
+      </c>
+      <c r="B29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
+        <v>34</v>
+      </c>
+      <c r="B33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
+        <v>35</v>
+      </c>
+      <c r="B34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
+        <v>36</v>
+      </c>
+      <c r="B35" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
+        <v>37</v>
+      </c>
+      <c r="B36" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
+        <v>39</v>
+      </c>
+      <c r="B38" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
+        <v>40</v>
+      </c>
+      <c r="B39" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
+        <v>41</v>
+      </c>
+      <c r="B40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
+        <v>42</v>
+      </c>
+      <c r="B41" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
+        <v>43</v>
+      </c>
+      <c r="B42" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
+        <v>44</v>
+      </c>
+      <c r="B43" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
+        <v>45</v>
+      </c>
+      <c r="B44" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
+        <v>46</v>
+      </c>
+      <c r="B45" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
+        <v>47</v>
+      </c>
+      <c r="B46" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
+        <v>48</v>
+      </c>
+      <c r="B47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
+        <v>49</v>
+      </c>
+      <c r="B48" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+      <c r="B49" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>